<commit_message>
[web]  - [`saveTitle(var`)]: **NEW** command to save the current page title to a variable.  - supports the `partialLinkText` locator (alias: `partial`).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_function.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_function.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lium183/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A68BE-B953-974A-9DB8-2FD4FC12B7FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3E3DA7-16B2-9D46-9349-31B97BB54AF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17080" yWindow="-28340" windowWidth="34120" windowHeight="28340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,11 +57,12 @@
     <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="757">
   <si>
     <t>target</t>
   </si>
@@ -2307,29 +2308,59 @@
     <t>v5-epoch</t>
   </si>
   <si>
-    <t>$(date|format|${v4}|MM/dd/yyyy HH:mm:ss.S|epoch)</t>
-  </si>
-  <si>
-    <t>$(date|format|${v5}|MM/dd/yyyy HH:mm:ss.S|epoch)</t>
-  </si>
-  <si>
-    <t>[NUMBER(${v4-epoch}) =&gt; minus(${v5-epoch}) abs]</t>
-  </si>
-  <si>
     <t>convert to timestamp</t>
   </si>
   <si>
-    <t>do the math</t>
-  </si>
-  <si>
     <t>[NUMBER(${v5-epoch}) =&gt; minus(${v4-epoch})]</t>
+  </si>
+  <si>
+    <t>MM/dd/yyyy HH:mm:ss.S</t>
+  </si>
+  <si>
+    <t>[NUMBER([DATE(${v4},${dateformat}) =&gt; format(epoch)]) =&gt; minus([DATE(${v5},${dateformat}) =&gt; format(epoch)]) abs]</t>
+  </si>
+  <si>
+    <t>dateformat</t>
+  </si>
+  <si>
+    <t>do the math, take 1</t>
+  </si>
+  <si>
+    <t>$(date|format|${v4}|${dateformat}|epoch)</t>
+  </si>
+  <si>
+    <r>
+      <t>$(date|format|${v5}|</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>${dateformat}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>|epoch)</t>
+    </r>
+  </si>
+  <si>
+    <t>do it again, take 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2405,6 +2436,25 @@
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2469,7 +2519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2625,6 +2675,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5018,11 +5076,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O321"/>
+  <dimension ref="A1:O320"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6473,9 +6531,7 @@
     </row>
     <row r="55" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
-      <c r="B55" s="21" t="s">
-        <v>751</v>
-      </c>
+      <c r="B55" s="21"/>
       <c r="C55" s="22" t="s">
         <v>5</v>
       </c>
@@ -6483,10 +6539,10 @@
         <v>319</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="G55" s="36"/>
       <c r="H55" s="23"/>
@@ -6500,7 +6556,9 @@
     </row>
     <row r="56" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
-      <c r="B56" s="21"/>
+      <c r="B56" s="21" t="s">
+        <v>748</v>
+      </c>
       <c r="C56" s="22" t="s">
         <v>5</v>
       </c>
@@ -6508,12 +6566,12 @@
         <v>319</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>749</v>
-      </c>
-      <c r="G56" s="23"/>
+        <v>754</v>
+      </c>
+      <c r="G56" s="36"/>
       <c r="H56" s="23"/>
       <c r="I56" s="30"/>
       <c r="J56" s="35"/>
@@ -6525,20 +6583,18 @@
     </row>
     <row r="57" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
-      <c r="B57" s="21" t="s">
-        <v>752</v>
-      </c>
+      <c r="B57" s="21"/>
       <c r="C57" s="22" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>75</v>
+        <v>319</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>745</v>
-      </c>
-      <c r="F57" s="23" t="s">
-        <v>753</v>
+        <v>747</v>
+      </c>
+      <c r="F57" s="46" t="s">
+        <v>755</v>
       </c>
       <c r="G57" s="23"/>
       <c r="H57" s="23"/>
@@ -6552,23 +6608,23 @@
     </row>
     <row r="58" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
-      <c r="B58" s="15" t="s">
-        <v>752</v>
-      </c>
-      <c r="C58" s="29" t="s">
+      <c r="B58" s="21" t="s">
+        <v>753</v>
+      </c>
+      <c r="C58" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="30" t="s">
+      <c r="E58" s="23" t="s">
         <v>745</v>
       </c>
-      <c r="F58" s="30" t="s">
-        <v>750</v>
-      </c>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
+      <c r="F58" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
       <c r="I58" s="30"/>
       <c r="J58" s="35"/>
       <c r="K58" s="17"/>
@@ -6579,11 +6635,21 @@
     </row>
     <row r="59" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
+      <c r="B59" s="47" t="s">
+        <v>756</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E59" s="30" t="s">
+        <v>745</v>
+      </c>
+      <c r="F59" s="30" t="s">
+        <v>751</v>
+      </c>
       <c r="G59" s="30"/>
       <c r="H59" s="30"/>
       <c r="I59" s="30"/>
@@ -11031,23 +11097,6 @@
       <c r="N320" s="18"/>
       <c r="O320" s="17"/>
     </row>
-    <row r="321" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A321" s="14"/>
-      <c r="B321" s="15"/>
-      <c r="C321" s="29"/>
-      <c r="D321" s="30"/>
-      <c r="E321" s="30"/>
-      <c r="F321" s="30"/>
-      <c r="G321" s="30"/>
-      <c r="H321" s="30"/>
-      <c r="I321" s="30"/>
-      <c r="J321" s="35"/>
-      <c r="K321" s="17"/>
-      <c r="L321" s="18"/>
-      <c r="M321" s="16"/>
-      <c r="N321" s="18"/>
-      <c r="O321" s="17"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -11056,18 +11105,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N122:N321">
+  <conditionalFormatting sqref="N3:N320">
     <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
-      <formula>LEFT(N122,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N3,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
-      <formula>LEFT(N122,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N3,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
-      <formula>LEFT(N122,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N3,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N121 N322:N1048576">
+  <conditionalFormatting sqref="N1 N321:N1048576">
     <cfRule type="beginsWith" dxfId="8" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -11078,11 +11127,11 @@
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C321" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C320" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D321" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D320" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>